<commit_message>
Update excel-based upload files
</commit_message>
<xml_diff>
--- a/tests/spreadsheet_files/excel 2007.xlsx
+++ b/tests/spreadsheet_files/excel 2007.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancahearn/software/benefits-studio/gns/notifications-admin/tests/spreadsheet_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA93E14-D43E-8C47-87BD-E7EB89E03E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="24740" yWindow="500" windowWidth="24760" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -42,12 +48,6 @@
     <t>tomato</t>
   </si>
   <si>
-    <t>07739 468 050</t>
-  </si>
-  <si>
-    <t>07527 125 974</t>
-  </si>
-  <si>
     <t>Not Pete</t>
   </si>
   <si>
@@ -57,9 +57,6 @@
     <t>Avacado</t>
   </si>
   <si>
-    <t>07512 058 823</t>
-  </si>
-  <si>
     <t>Still Not Pete</t>
   </si>
   <si>
@@ -67,12 +64,21 @@
   </si>
   <si>
     <t>Pear</t>
+  </si>
+  <si>
+    <t>202 946 8050</t>
+  </si>
+  <si>
+    <t>202 712 5974</t>
+  </si>
+  <si>
+    <t>202 205 8823</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,6 +116,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -434,18 +448,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,9 +475,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -473,32 +489,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>